<commit_message>
Fixed some issues with the scraping. Added Spartan results to OCR Series
</commit_message>
<xml_diff>
--- a/RaceWebScraper/data/LigaOCRA/7 - KongRace-Polinya-2024.xlsx
+++ b/RaceWebScraper/data/LigaOCRA/7 - KongRace-Polinya-2024.xlsx
@@ -19,8 +19,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[HH]:MM:SS.000"/>
+    <numFmt numFmtId="165" formatCode="#.#"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -54,10 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -503,7 +505,7 @@
       <c r="F2" s="2" t="n">
         <v>0.03540509259259259</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="3" t="n">
         <v>100</v>
       </c>
     </row>
@@ -534,9 +536,9 @@
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.03719907407407407</v>
-      </c>
-      <c r="G3" t="n">
+        <v>0.0371875</v>
+      </c>
+      <c r="G3" s="3" t="n">
         <v>92</v>
       </c>
     </row>
@@ -567,9 +569,9 @@
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.04163194444444444</v>
-      </c>
-      <c r="G4" t="n">
+        <v>0.0416087962962963</v>
+      </c>
+      <c r="G4" s="3" t="n">
         <v>86</v>
       </c>
     </row>
@@ -600,9 +602,9 @@
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.04351851851851852</v>
-      </c>
-      <c r="G5" t="n">
+        <v>0.04350694444444445</v>
+      </c>
+      <c r="G5" s="3" t="n">
         <v>82</v>
       </c>
     </row>
@@ -633,9 +635,9 @@
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.04423611111111111</v>
-      </c>
-      <c r="G6" t="n">
+        <v>0.04421296296296296</v>
+      </c>
+      <c r="G6" s="3" t="n">
         <v>80</v>
       </c>
     </row>
@@ -666,9 +668,9 @@
         </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.04701388888888889</v>
-      </c>
-      <c r="G7" t="n">
+        <v>0.04699074074074074</v>
+      </c>
+      <c r="G7" s="3" t="n">
         <v>79</v>
       </c>
     </row>
@@ -694,12 +696,8 @@
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
+      <c r="F8" s="2" t="inlineStr"/>
+      <c r="G8" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -725,12 +723,8 @@
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
+      <c r="F9" s="2" t="inlineStr"/>
+      <c r="G9" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -756,12 +750,8 @@
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
+      <c r="F10" s="2" t="inlineStr"/>
+      <c r="G10" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -787,12 +777,8 @@
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
+      <c r="F11" s="2" t="inlineStr"/>
+      <c r="G11" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -818,12 +804,8 @@
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
+      <c r="F12" s="2" t="inlineStr"/>
+      <c r="G12" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -849,12 +831,8 @@
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
+      <c r="F13" s="2" t="inlineStr"/>
+      <c r="G13" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -880,12 +858,8 @@
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
+      <c r="F14" s="2" t="inlineStr"/>
+      <c r="G14" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -911,12 +885,8 @@
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
+      <c r="F15" s="2" t="inlineStr"/>
+      <c r="G15" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -942,12 +912,8 @@
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
+      <c r="F16" s="2" t="inlineStr"/>
+      <c r="G16" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -973,12 +939,8 @@
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
+      <c r="F17" s="2" t="inlineStr"/>
+      <c r="G17" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1004,12 +966,8 @@
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
+      <c r="F18" s="2" t="inlineStr"/>
+      <c r="G18" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1035,12 +993,8 @@
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
+      <c r="F19" s="2" t="inlineStr"/>
+      <c r="G19" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1128,12 +1082,8 @@
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
+      <c r="F2" s="2" t="inlineStr"/>
+      <c r="G2" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1159,12 +1109,8 @@
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
+      <c r="F3" s="2" t="inlineStr"/>
+      <c r="G3" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1190,12 +1136,8 @@
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
+      <c r="F4" s="2" t="inlineStr"/>
+      <c r="G4" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1221,12 +1163,8 @@
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
+      <c r="F5" s="2" t="inlineStr"/>
+      <c r="G5" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1252,12 +1190,8 @@
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
+      <c r="F6" s="2" t="inlineStr"/>
+      <c r="G6" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1283,12 +1217,8 @@
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
+      <c r="F7" s="2" t="inlineStr"/>
+      <c r="G7" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1381,9 +1311,9 @@
         </is>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.04193287037037037</v>
-      </c>
-      <c r="G2" t="n">
+        <v>0.04190972222222222</v>
+      </c>
+      <c r="G2" s="3" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1414,10 +1344,10 @@
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.04641203703703704</v>
-      </c>
-      <c r="G3" t="n">
-        <v>90.3</v>
+        <v>0.04640046296296296</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>90.322</v>
       </c>
     </row>
     <row r="4">
@@ -1449,8 +1379,8 @@
       <c r="F4" s="2" t="n">
         <v>0.04768518518518518</v>
       </c>
-      <c r="G4" t="n">
-        <v>87.90000000000001</v>
+      <c r="G4" s="3" t="n">
+        <v>87.88800000000001</v>
       </c>
     </row>
     <row r="5">
@@ -1480,10 +1410,10 @@
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.04850694444444444</v>
-      </c>
-      <c r="G5" t="n">
-        <v>86.40000000000001</v>
+        <v>0.0484837962962963</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>86.441</v>
       </c>
     </row>
     <row r="6">
@@ -1513,10 +1443,10 @@
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.04983796296296297</v>
-      </c>
-      <c r="G6" t="n">
-        <v>84.09999999999999</v>
+        <v>0.04982638888888889</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>84.111</v>
       </c>
     </row>
     <row r="7">
@@ -1548,8 +1478,8 @@
       <c r="F7" s="2" t="n">
         <v>0.05082175925925926</v>
       </c>
-      <c r="G7" t="n">
-        <v>82.5</v>
+      <c r="G7" s="3" t="n">
+        <v>82.464</v>
       </c>
     </row>
     <row r="8">
@@ -1579,10 +1509,10 @@
         </is>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.05251157407407407</v>
-      </c>
-      <c r="G8" t="n">
-        <v>79.90000000000001</v>
+        <v>0.0525</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>79.828</v>
       </c>
     </row>
     <row r="9">
@@ -1612,10 +1542,10 @@
         </is>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.05280092592592592</v>
-      </c>
-      <c r="G9" t="n">
-        <v>79.40000000000001</v>
+        <v>0.05278935185185185</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>79.39</v>
       </c>
     </row>
     <row r="10">
@@ -1645,10 +1575,10 @@
         </is>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.05451388888888889</v>
-      </c>
-      <c r="G10" t="n">
-        <v>76.90000000000001</v>
+        <v>0.05449074074074074</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>76.91200000000001</v>
       </c>
     </row>
     <row r="11">
@@ -1678,10 +1608,10 @@
         </is>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.05571759259259259</v>
-      </c>
-      <c r="G11" t="n">
-        <v>75.3</v>
+        <v>0.05569444444444444</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>75.249</v>
       </c>
     </row>
     <row r="12">
@@ -1711,10 +1641,10 @@
         </is>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.05665509259259259</v>
-      </c>
-      <c r="G12" t="n">
-        <v>74</v>
+        <v>0.05662037037037037</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>74.01900000000001</v>
       </c>
     </row>
     <row r="13">
@@ -1744,10 +1674,10 @@
         </is>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0.0572337962962963</v>
-      </c>
-      <c r="G13" t="n">
-        <v>73.3</v>
+        <v>0.05719907407407408</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>73.27</v>
       </c>
     </row>
     <row r="14">
@@ -1777,183 +1707,173 @@
         </is>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0.0593287037037037</v>
-      </c>
-      <c r="G14" t="n">
-        <v>70.7</v>
+        <v>0.05927083333333334</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>70.709</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>918</t>
+          <t>745</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>OCHANDO HURTADO CARLOS</t>
+          <t>DOMINGO UBEDA DANIEL</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>UNITTEAM</t>
+          <t>VB SPORT</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>GGEE 45-49 M</t>
+          <t>GGEE 40-44 M</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0.06822916666666666</v>
-      </c>
-      <c r="G15" t="n">
-        <v>61.5</v>
+        <v>0.06435185185185185</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>65.126</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>918</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MORENO MARTIN SANTI</t>
+          <t>OCHANDO HURTADO CARLOS</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CROSSFIT QB</t>
+          <t>UNITTEAM</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>GGEE 35-39 M</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
-        <v>0</v>
+          <t>GGEE 45-49 M</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>0.06819444444444445</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>61.456</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>116</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>GáMEZ SOLA ALEJANDRO</t>
+          <t>MORENO MARTIN SANTI</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>QB CROSSFIT</t>
+          <t>CROSSFIT QB</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>GGEE 40-44 M</t>
+          <t>GGEE 35-39 M</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
+      <c r="F17" s="2" t="inlineStr"/>
+      <c r="G17" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LLORT BARAIBAR LUIS MIGUEL</t>
+          <t>GáMEZ SOLA ALEJANDRO</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>THUNDER RACERS</t>
+          <t>QB CROSSFIT</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>GGEE 35-39 M</t>
+          <t>GGEE 40-44 M</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
+      <c r="F18" s="2" t="inlineStr"/>
+      <c r="G18" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>182</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>GARCIA LIRIA VICTOR</t>
+          <t>LLORT BARAIBAR LUIS MIGUEL</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>BARRAKONG</t>
+          <t>THUNDER RACERS</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>GGEE 40-44 M</t>
+          <t>GGEE 35-39 M</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
+      <c r="F19" s="2" t="inlineStr"/>
+      <c r="G19" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>302</t>
+          <t>232</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MOTA ROVIRA SERGI</t>
+          <t>GARCIA LIRIA VICTOR</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>TEAM XXX BLACK MAMBA</t>
+          <t>BARRAKONG</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1962,184 +1882,160 @@
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
+      <c r="F20" s="2" t="inlineStr"/>
+      <c r="G20" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>334</t>
+          <t>302</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BORDES GARCIA XAVIER</t>
+          <t>MOTA ROVIRA SERGI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>INDEPENDIENTE</t>
+          <t>TEAM XXX BLACK MAMBA</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>GGEE 30-34 M</t>
+          <t>GGEE 40-44 M</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
+      <c r="F21" s="2" t="inlineStr"/>
+      <c r="G21" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>383</t>
+          <t>334</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>HOEKSTRA ARJAN</t>
+          <t>BORDES GARCIA XAVIER</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OUTDOOR CIRCUIT</t>
+          <t>INDEPENDIENTE</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>GGEE 50-54 M</t>
+          <t>GGEE 30-34 M</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
+      <c r="F22" s="2" t="inlineStr"/>
+      <c r="G22" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>415</t>
+          <t>383</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SARDINÉ CARBONÉS PAU</t>
+          <t>HOEKSTRA ARJAN</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SPARRACS TEAM</t>
+          <t>OUTDOOR CIRCUIT</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>GGEE 40-44 M</t>
+          <t>GGEE 50-54 M</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G23" t="n">
+      <c r="F23" s="2" t="inlineStr"/>
+      <c r="G23" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>423</t>
+          <t>415</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>GASTON ARQUES MARC</t>
+          <t>SARDINÉ CARBONÉS PAU</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>TEAMDESTROYER</t>
+          <t>SPARRACS TEAM</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>GGEE 30-34 M</t>
+          <t>GGEE 40-44 M</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
-      <c r="F24" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
+      <c r="F24" s="2" t="inlineStr"/>
+      <c r="G24" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>424</t>
+          <t>423</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PRAT VERICAT JORDI</t>
+          <t>GASTON ARQUES MARC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>TEAM XXX BLACK MAMBA</t>
+          <t>TEAMDESTROYER</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>GGEE 40-44 M</t>
+          <t>GGEE 30-34 M</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
+      <c r="F25" s="2" t="inlineStr"/>
+      <c r="G25" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>427</t>
+          <t>424</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MARTíNEZ MOLINA FRANCISCO JAVIER</t>
+          <t>PRAT VERICAT JORDI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>UNIT-TEAM</t>
+          <t>TEAM XXX BLACK MAMBA</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2148,122 +2044,106 @@
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G26" t="n">
+      <c r="F26" s="2" t="inlineStr"/>
+      <c r="G26" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>448</t>
+          <t>427</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MORENO MARTINEZ XAVIER</t>
+          <t>MARTíNEZ MOLINA FRANCISCO JAVIER</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OLLLU RACERS</t>
+          <t>UNIT-TEAM</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>GGEE 30-34 M</t>
+          <t>GGEE 40-44 M</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
-      <c r="F27" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G27" t="n">
+      <c r="F27" s="2" t="inlineStr"/>
+      <c r="G27" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>448</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MOLINé JESúS</t>
+          <t>MORENO MARTINEZ XAVIER</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>THUNDER RACERS</t>
+          <t>OLLLU RACERS</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>GGEE 40-44 M</t>
+          <t>GGEE 30-34 M</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G28" t="n">
+      <c r="F28" s="2" t="inlineStr"/>
+      <c r="G28" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>450</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SAEZ SERRA MARC</t>
+          <t>MOLINé JESúS</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>TEAM DESTROYER</t>
+          <t>THUNDER RACERS</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>GGEE 25-29 M</t>
+          <t>GGEE 40-44 M</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G29" t="n">
+      <c r="F29" s="2" t="inlineStr"/>
+      <c r="G29" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>515</t>
+          <t>456</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CORA RAUL</t>
+          <t>SAEZ SERRA MARC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>UNIT TEAM</t>
+          <t>TEAM DESTROYER</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2272,184 +2152,160 @@
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
-      <c r="F30" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G30" t="n">
+      <c r="F30" s="2" t="inlineStr"/>
+      <c r="G30" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>520</t>
+          <t>515</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>JESúS HERNáNDEZ DAVID</t>
+          <t>CORA RAUL</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>THUNDER RACERS</t>
+          <t>UNIT TEAM</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>GGEE 50-54 M</t>
+          <t>GGEE 25-29 M</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
-      <c r="F31" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G31" t="n">
+      <c r="F31" s="2" t="inlineStr"/>
+      <c r="G31" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>524</t>
+          <t>520</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>PEREZ ALUART AARON</t>
+          <t>JESúS HERNáNDEZ DAVID</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>FOT-LIFIT</t>
+          <t>THUNDER RACERS</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>GGEE 20-24 M</t>
+          <t>GGEE 50-54 M</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
-      <c r="F32" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
+      <c r="F32" s="2" t="inlineStr"/>
+      <c r="G32" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>530</t>
+          <t>524</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>GONZáLEZ ARRABAL ANTONIO</t>
+          <t>PEREZ ALUART AARON</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>UNIT TEAM</t>
+          <t>FOT-LIFIT</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>GGEE +60 M</t>
+          <t>GGEE 20-24 M</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G33" t="n">
+      <c r="F33" s="2" t="inlineStr"/>
+      <c r="G33" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>552</t>
+          <t>530</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>VERDAGUER RUIZ MARC</t>
+          <t>GONZáLEZ ARRABAL ANTONIO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>FOTLI</t>
+          <t>UNIT TEAM</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>GGEE 40-44 M</t>
+          <t>GGEE +60 M</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
-      <c r="F34" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G34" t="n">
+      <c r="F34" s="2" t="inlineStr"/>
+      <c r="G34" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>555</t>
+          <t>552</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>BERGADà LASECA FREDERIC</t>
+          <t>VERDAGUER RUIZ MARC</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PERCUTEAM</t>
+          <t>FOTLI</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>GGEE 35-39 M</t>
+          <t>GGEE 40-44 M</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
-      <c r="F35" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G35" t="n">
+      <c r="F35" s="2" t="inlineStr"/>
+      <c r="G35" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>593</t>
+          <t>555</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>COLL VILA EDUARD</t>
+          <t>BERGADà LASECA FREDERIC</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OLLU RACERS</t>
+          <t>PERCUTEAM</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2458,29 +2314,25 @@
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
-      <c r="F36" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G36" t="n">
+      <c r="F36" s="2" t="inlineStr"/>
+      <c r="G36" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>619</t>
+          <t>593</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ADSUARA CANOS JOSE PASCUAL</t>
+          <t>COLL VILA EDUARD</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>BETXí CROSS TRAINING</t>
+          <t>OLLU RACERS</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2489,74 +2341,62 @@
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
-      <c r="F37" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G37" t="n">
+      <c r="F37" s="2" t="inlineStr"/>
+      <c r="G37" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>728</t>
+          <t>619</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>PADILLA VILASECA ASIER</t>
+          <t>ADSUARA CANOS JOSE PASCUAL</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BARRAKONG</t>
+          <t>BETXí CROSS TRAINING</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>SUB 20M</t>
+          <t>GGEE 35-39 M</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
-      <c r="F38" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G38" t="n">
+      <c r="F38" s="2" t="inlineStr"/>
+      <c r="G38" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>745</t>
+          <t>728</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>DOMINGO UBEDA DANIEL</t>
+          <t>PADILLA VILASECA ASIER</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>VB SPORT</t>
+          <t>BARRAKONG</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>GGEE 40-44 M</t>
+          <t>SUB 20M</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G39" t="n">
+      <c r="F39" s="2" t="inlineStr"/>
+      <c r="G39" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2582,12 +2422,8 @@
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
-      <c r="F40" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G40" t="n">
+      <c r="F40" s="2" t="inlineStr"/>
+      <c r="G40" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2613,12 +2449,8 @@
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
-      <c r="F41" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G41" t="n">
+      <c r="F41" s="2" t="inlineStr"/>
+      <c r="G41" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2644,12 +2476,8 @@
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
-      <c r="F42" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G42" t="n">
+      <c r="F42" s="2" t="inlineStr"/>
+      <c r="G42" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2675,12 +2503,8 @@
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G43" t="n">
+      <c r="F43" s="2" t="inlineStr"/>
+      <c r="G43" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2706,12 +2530,8 @@
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
-      <c r="F44" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G44" t="n">
+      <c r="F44" s="2" t="inlineStr"/>
+      <c r="G44" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2737,12 +2557,8 @@
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
-      <c r="F45" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G45" t="n">
+      <c r="F45" s="2" t="inlineStr"/>
+      <c r="G45" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2768,12 +2584,8 @@
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G46" t="n">
+      <c r="F46" s="2" t="inlineStr"/>
+      <c r="G46" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2799,12 +2611,8 @@
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
-      <c r="F47" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G47" t="n">
+      <c r="F47" s="2" t="inlineStr"/>
+      <c r="G47" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2830,12 +2638,8 @@
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G48" t="n">
+      <c r="F48" s="2" t="inlineStr"/>
+      <c r="G48" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2861,12 +2665,8 @@
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
-      <c r="F49" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G49" t="n">
+      <c r="F49" s="2" t="inlineStr"/>
+      <c r="G49" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2892,12 +2692,8 @@
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G50" t="n">
+      <c r="F50" s="2" t="inlineStr"/>
+      <c r="G50" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2923,12 +2719,8 @@
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
-      <c r="F51" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G51" t="n">
+      <c r="F51" s="2" t="inlineStr"/>
+      <c r="G51" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2954,12 +2746,8 @@
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
-      <c r="F52" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G52" t="n">
+      <c r="F52" s="2" t="inlineStr"/>
+      <c r="G52" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2985,12 +2773,8 @@
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
-      <c r="F53" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G53" t="n">
+      <c r="F53" s="2" t="inlineStr"/>
+      <c r="G53" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3016,12 +2800,8 @@
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
-      <c r="F54" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G54" t="n">
+      <c r="F54" s="2" t="inlineStr"/>
+      <c r="G54" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3047,12 +2827,8 @@
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
-      <c r="F55" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G55" t="n">
+      <c r="F55" s="2" t="inlineStr"/>
+      <c r="G55" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3078,12 +2854,8 @@
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
-      <c r="F56" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G56" t="n">
+      <c r="F56" s="2" t="inlineStr"/>
+      <c r="G56" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3109,12 +2881,8 @@
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
-      <c r="F57" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G57" t="n">
+      <c r="F57" s="2" t="inlineStr"/>
+      <c r="G57" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3140,12 +2908,8 @@
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
-      <c r="F58" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G58" t="n">
+      <c r="F58" s="2" t="inlineStr"/>
+      <c r="G58" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3171,12 +2935,8 @@
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
-      <c r="F59" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G59" t="n">
+      <c r="F59" s="2" t="inlineStr"/>
+      <c r="G59" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3202,12 +2962,8 @@
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
-      <c r="F60" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G60" t="n">
+      <c r="F60" s="2" t="inlineStr"/>
+      <c r="G60" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3233,12 +2989,8 @@
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
-      <c r="F61" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G61" t="n">
+      <c r="F61" s="2" t="inlineStr"/>
+      <c r="G61" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3264,12 +3016,8 @@
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
-      <c r="F62" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G62" t="n">
+      <c r="F62" s="2" t="inlineStr"/>
+      <c r="G62" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3357,12 +3105,8 @@
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
+      <c r="F2" s="2" t="inlineStr"/>
+      <c r="G2" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3388,12 +3132,8 @@
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
+      <c r="F3" s="2" t="inlineStr"/>
+      <c r="G3" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3419,12 +3159,8 @@
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
+      <c r="F4" s="2" t="inlineStr"/>
+      <c r="G4" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3450,12 +3186,8 @@
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
+      <c r="F5" s="2" t="inlineStr"/>
+      <c r="G5" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3481,12 +3213,8 @@
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
+      <c r="F6" s="2" t="inlineStr"/>
+      <c r="G6" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3512,12 +3240,8 @@
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
+      <c r="F7" s="2" t="inlineStr"/>
+      <c r="G7" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3543,12 +3267,8 @@
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
+      <c r="F8" s="2" t="inlineStr"/>
+      <c r="G8" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3574,12 +3294,8 @@
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
+      <c r="F9" s="2" t="inlineStr"/>
+      <c r="G9" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3605,12 +3321,8 @@
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
+      <c r="F10" s="2" t="inlineStr"/>
+      <c r="G10" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3636,12 +3348,8 @@
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
+      <c r="F11" s="2" t="inlineStr"/>
+      <c r="G11" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3667,12 +3375,8 @@
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
+      <c r="F12" s="2" t="inlineStr"/>
+      <c r="G12" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3698,12 +3402,8 @@
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
+      <c r="F13" s="2" t="inlineStr"/>
+      <c r="G13" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3729,12 +3429,8 @@
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" s="2" t="inlineStr">
-        <is>
-          <t>Descalificado</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
+      <c r="F14" s="2" t="inlineStr"/>
+      <c r="G14" s="3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>